<commit_message>
Update 10/02, up to date with run 30
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_ELC_CO2BND.xlsx
+++ b/SuppXLS/Scen_ELC_CO2BND.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\Veda_models\KModel_04\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B76FD2E3-581C-4AF1-9304-38C02B4C1283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32172CE4-F08A-4ADF-8FDC-27DB5F9EBB90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5328" yWindow="3720" windowWidth="15336" windowHeight="8040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UC_CO2" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t>Pset_CI</t>
   </si>
@@ -757,10 +757,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AK33"/>
+  <dimension ref="A1:AK32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="E3" zoomScale="70" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -865,11 +865,11 @@
         <v>26</v>
       </c>
       <c r="E7">
-        <v>2022</v>
+        <v>2030</v>
       </c>
       <c r="G7" s="2">
-        <f>E19*(1-Q7)</f>
-        <v>796.71332927570995</v>
+        <f>E18*(1-Q7)</f>
+        <v>210</v>
       </c>
       <c r="N7" t="s">
         <v>20</v>
@@ -887,17 +887,17 @@
         <v>26</v>
       </c>
       <c r="E8">
-        <v>2030</v>
+        <v>2040</v>
       </c>
       <c r="G8" s="2">
-        <f>E19*(1-Q8)</f>
-        <v>682.89713937917998</v>
+        <f>E18*(1-Q8)</f>
+        <v>120</v>
       </c>
       <c r="N8" t="s">
         <v>20</v>
       </c>
       <c r="Q8" s="4">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="R8" s="4"/>
     </row>
@@ -909,16 +909,35 @@
         <v>26</v>
       </c>
       <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>15</v>
+        <v>2050</v>
+      </c>
+      <c r="G9" s="2">
+        <f>E18*(1-Q9)</f>
+        <v>29.999999999999993</v>
       </c>
       <c r="N9" t="s">
         <v>20</v>
       </c>
+      <c r="Q9" s="4">
+        <v>0.9</v>
+      </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>15</v>
+      </c>
+      <c r="N10" t="s">
+        <v>20</v>
+      </c>
       <c r="U10" s="5"/>
       <c r="AB10" s="6"/>
       <c r="AC10" s="7"/>
@@ -966,61 +985,71 @@
       <c r="B17" t="s">
         <v>12</v>
       </c>
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17">
+        <v>2030</v>
+      </c>
+      <c r="F17">
+        <v>2006</v>
+      </c>
+      <c r="G17">
+        <v>2010</v>
+      </c>
+      <c r="H17">
+        <v>2020</v>
+      </c>
+      <c r="I17">
+        <v>2025</v>
+      </c>
+      <c r="J17">
+        <v>2030</v>
+      </c>
+      <c r="K17">
+        <v>2035</v>
+      </c>
+      <c r="L17">
+        <v>2040</v>
+      </c>
+      <c r="M17">
+        <v>2045</v>
+      </c>
+      <c r="N17">
+        <v>2050</v>
+      </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18">
-        <v>2022</v>
-      </c>
-      <c r="F18">
-        <v>2006</v>
-      </c>
-      <c r="G18">
-        <v>2010</v>
-      </c>
-      <c r="H18">
-        <v>2020</v>
-      </c>
-      <c r="I18">
-        <v>2025</v>
-      </c>
-      <c r="J18">
-        <v>2030</v>
-      </c>
-      <c r="K18">
-        <v>2035</v>
-      </c>
-      <c r="L18">
-        <v>2040</v>
-      </c>
-      <c r="M18">
-        <v>2045</v>
-      </c>
-      <c r="N18">
-        <v>2050</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="E18" s="2">
+        <v>300</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>29</v>
       </c>
-      <c r="C19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19" s="2">
-        <v>1138.1618989653</v>
-      </c>
+      <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
@@ -1032,7 +1061,9 @@
       <c r="N19" s="2"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="E20" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
@@ -1044,9 +1075,7 @@
       <c r="N20" s="2"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="E21" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -1153,110 +1182,98 @@
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="C31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" s="2">
+        <f>SUM(E18:E23)</f>
+        <v>300</v>
+      </c>
+      <c r="F31" s="2">
+        <f t="shared" ref="F31:N31" si="0">SUM(F18:F23)</f>
+        <v>0</v>
+      </c>
+      <c r="G31" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H31" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I31" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J31" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K31" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L31" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M31" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N31" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C32" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D32" t="s">
         <v>19</v>
       </c>
       <c r="E32" s="2">
-        <f>SUM(E19:E24)</f>
-        <v>1138.1618989653</v>
+        <f>SUM(E24:E29)</f>
+        <v>0</v>
       </c>
       <c r="F32" s="2">
-        <f t="shared" ref="F32:N32" si="0">SUM(F19:F24)</f>
+        <f t="shared" ref="F32:N32" si="1">SUM(F24:F29)</f>
         <v>0</v>
       </c>
       <c r="G32" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H32" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I32" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J32" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K32" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L32" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M32" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N32" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C33" t="s">
-        <v>9</v>
-      </c>
-      <c r="D33" t="s">
-        <v>19</v>
-      </c>
-      <c r="E33" s="2">
-        <f>SUM(E25:E30)</f>
-        <v>0</v>
-      </c>
-      <c r="F33" s="2">
-        <f t="shared" ref="F33:N33" si="1">SUM(F25:F30)</f>
-        <v>0</v>
-      </c>
-      <c r="G33" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H33" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I33" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J33" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K33" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L33" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M33" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N33" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>

</xml_diff>